<commit_message>
Committing some data sets
</commit_message>
<xml_diff>
--- a/minjava/r2_100.xlsx
+++ b/minjava/r2_100.xlsx
@@ -15,7 +15,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
   <si>
     <t>Hawaii</t>
   </si>
@@ -424,560 +436,560 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.4980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <v>7</v>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>0.83</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.66</v>
+        <v>0.83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.51</v>
+        <v>0.66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.705</v>
+        <v>0.51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.87</v>
+        <v>0.705</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.995</v>
+        <v>0.87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.51</v>
+        <v>0.995</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.28</v>
+        <v>0.51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.755</v>
+        <v>0.28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.09</v>
+        <v>0.755</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.67</v>
+        <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="D14" s="0" t="n">
-        <v>0.41</v>
+        <v>0.67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0.295</v>
+        <v>0.41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0.875</v>
+        <v>0.295</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.06</v>
+        <v>0.875</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.75</v>
+        <v>0.06</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0.615</v>
+        <v>0.75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0.585</v>
+        <v>0.615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.84</v>
+        <v>0.585</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>0.215</v>
+        <v>0.84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.08</v>
+        <v>0.215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.96</v>
+        <v>0.08</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.155</v>
+        <v>0.96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.4</v>
+        <v>0.155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>0.205</v>
+        <v>0.4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0.435</v>
+        <v>0.205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>0.98</v>
+        <v>0.435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.35</v>
+        <v>0.98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.445</v>
+        <v>0.35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.715</v>
+        <v>0.445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>0.54</v>
+        <v>0.715</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>0.815</v>
+        <v>0.54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>0.505</v>
+        <v>0.815</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.855</v>
+        <v>0.505</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.745</v>
+        <v>0.855</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.545</v>
+        <v>0.745</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.12</v>
+        <v>0.545</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="40">
@@ -985,13 +997,13 @@
         <v>15</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0.76</v>
+        <v>0.12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="41">
@@ -999,458 +1011,458 @@
         <v>19</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>0.415</v>
+        <v>0.76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0.475</v>
+        <v>0.415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>0.71</v>
+        <v>0.475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>0.545</v>
+        <v>0.71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.815</v>
+        <v>0.545</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.085</v>
+        <v>0.815</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>0.575</v>
+        <v>0.085</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>0.455</v>
+        <v>0.575</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>0.135</v>
+        <v>0.455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>0.865</v>
+        <v>0.135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0.34</v>
+        <v>0.865</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.755</v>
+        <v>0.34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0.4</v>
+        <v>0.755</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>0.295</v>
+        <v>0.4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>0.39</v>
+        <v>0.295</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>0.285</v>
+        <v>0.39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>0.875</v>
+        <v>0.285</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>0.665</v>
+        <v>0.875</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>0.475</v>
+        <v>0.665</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>0.24</v>
+        <v>0.475</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>0.275</v>
+        <v>0.21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>0.365</v>
+        <v>0.275</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>0.63</v>
+        <v>0.365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>0.02</v>
+        <v>0.63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>0.94</v>
+        <v>0.02</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>0.975</v>
+        <v>0.94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>0.44</v>
+        <v>0.975</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>0.955</v>
+        <v>0.44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>0.335</v>
+        <v>0.955</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C71" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="D71" s="0" t="n">
-        <v>0.775</v>
+        <v>0.335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>0.18</v>
+        <v>0.775</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>0.18</v>
@@ -1458,349 +1470,349 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>0.335</v>
+        <v>0.18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>0.65</v>
+        <v>0.335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>0.355</v>
+        <v>0.65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>0.335</v>
+        <v>0.355</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>0.735</v>
+        <v>0.335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>0.33</v>
+        <v>0.735</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>0.425</v>
+        <v>0.33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>0.48</v>
+        <v>0.425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>0.035</v>
+        <v>0.48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>0.38</v>
+        <v>0.035</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>0.295</v>
+        <v>0.38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>0.03</v>
+        <v>0.295</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>0.66</v>
+        <v>0.03</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>0.225</v>
+        <v>0.66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>0.2</v>
+        <v>0.225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>0.155</v>
+        <v>0.03</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>0.38</v>
+        <v>0.155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>0.45</v>
+        <v>0.38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>0.69</v>
+        <v>0.45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>0.575</v>
+        <v>0.69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>0.5</v>
+        <v>0.575</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>0.945</v>
+        <v>0.95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>0.945</v>
@@ -1808,15 +1820,29 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
-        <v>22</v>
+        <v>108</v>
       </c>
       <c r="B99" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>0.945</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="100">
+      <c r="A100" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C99" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D99" s="0" t="n">
+      <c r="C100" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="0" t="n">
         <v>0.695</v>
       </c>
     </row>

</xml_diff>